<commit_message>
changed hardware to only use 2 PWMs instead of 4.
</commit_message>
<xml_diff>
--- a/outputs.xlsx
+++ b/outputs.xlsx
@@ -223,12 +223,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -244,6 +238,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,7 +542,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -554,125 +554,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7">
-        <v>4</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="C4" s="5">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7">
-        <v>4</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="C5" s="5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7">
-        <v>4</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="C6" s="5">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
@@ -680,193 +680,193 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>1</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>8</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="9">
-        <v>8</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="C12" s="7">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="9">
-        <v>8</v>
-      </c>
-      <c r="D13" s="9">
+      <c r="C13" s="7">
+        <v>8</v>
+      </c>
+      <c r="D13" s="7">
         <v>2</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="9">
-        <v>8</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="C14" s="7">
+        <v>8</v>
+      </c>
+      <c r="D14" s="7">
         <v>3</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="9">
-        <v>8</v>
-      </c>
-      <c r="D15" s="9">
-        <v>4</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="C15" s="7">
+        <v>8</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="9">
-        <v>8</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C16" s="7">
+        <v>8</v>
+      </c>
+      <c r="D16" s="7">
         <v>5</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="9">
-        <v>8</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="C17" s="7">
+        <v>8</v>
+      </c>
+      <c r="D17" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="9">
-        <v>8</v>
-      </c>
-      <c r="D18" s="9">
+      <c r="C18" s="7">
+        <v>8</v>
+      </c>
+      <c r="D18" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9">
-        <v>8</v>
-      </c>
-      <c r="D19" s="9">
+      <c r="C19" s="7">
+        <v>8</v>
+      </c>
+      <c r="D19" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="9">
-        <v>4</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="7">
+        <v>4</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="9">
-        <v>4</v>
-      </c>
-      <c r="D21" s="9">
+      <c r="C21" s="7">
+        <v>4</v>
+      </c>
+      <c r="D21" s="7">
         <v>2</v>
       </c>
       <c r="E21" t="s">
@@ -874,14 +874,14 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="9">
-        <v>4</v>
-      </c>
-      <c r="D22" s="9">
+      <c r="C22" s="7">
+        <v>4</v>
+      </c>
+      <c r="D22" s="7">
         <v>3</v>
       </c>
       <c r="E22" t="s">
@@ -889,14 +889,14 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="9">
-        <v>4</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="C23" s="7">
+        <v>4</v>
+      </c>
+      <c r="D23" s="7">
         <v>4</v>
       </c>
       <c r="E23" t="s">
@@ -907,13 +907,13 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="9">
-        <v>4</v>
-      </c>
-      <c r="D24" s="9">
+      <c r="C24" s="7">
+        <v>4</v>
+      </c>
+      <c r="D24" s="7">
         <v>1</v>
       </c>
       <c r="E24" t="s">
@@ -924,7 +924,7 @@
       <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C25" t="s">
@@ -941,16 +941,16 @@
       <c r="A26" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added winch.  still need to figure out channels etc.
</commit_message>
<xml_diff>
--- a/outputs.xlsx
+++ b/outputs.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="360" yWindow="45" windowWidth="20940" windowHeight="10110" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Outputs" sheetId="1" r:id="rId1"/>
+    <sheet name="Joysticks" sheetId="2" r:id="rId2"/>
+    <sheet name="Other Inputs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Hardware Summary</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>(Other Inputs)</t>
+  </si>
+  <si>
+    <t>winchMotor</t>
+  </si>
+  <si>
+    <t>Lift us up</t>
+  </si>
+  <si>
+    <t>winchSwitch</t>
+  </si>
+  <si>
+    <t>Do we want to turn on the winch motor?</t>
   </si>
 </sst>
 </file>
@@ -545,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,34 +673,36 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="7">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C8" s="7">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="7">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -700,7 +714,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>27</v>
@@ -715,10 +729,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -730,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>26</v>
@@ -745,10 +759,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -760,10 +774,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -775,7 +789,10 @@
         <v>8</v>
       </c>
       <c r="D14" s="7">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -787,42 +804,47 @@
         <v>8</v>
       </c>
       <c r="D15" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="7">
+        <v>8</v>
+      </c>
+      <c r="D16" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="E17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="E18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="E19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7"/>
@@ -834,7 +856,7 @@
     <row r="22" spans="1:5">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
@@ -843,6 +865,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7"/>
@@ -857,12 +880,18 @@
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1074,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1198,27 +1227,37 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7"/>
@@ -1253,6 +1292,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7"/>
@@ -1261,17 +1301,16 @@
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5">
+      <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7"/>
@@ -1279,6 +1318,13 @@
       <c r="C21" s="8"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
winch switch is on cyrpus module yo.
</commit_message>
<xml_diff>
--- a/outputs.xlsx
+++ b/outputs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>Hardware Summary</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Do we want to turn on the winch motor?</t>
+  </si>
+  <si>
+    <t>On Cyprus</t>
   </si>
 </sst>
 </file>
@@ -239,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -261,6 +264,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -560,7 +566,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,11 +667,11 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -678,11 +684,11 @@
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>8</v>
+      <c r="C7" s="7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>52</v>
@@ -1106,7 +1112,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1232,12 +1238,10 @@
       <c r="B8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="C8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="11"/>
       <c r="E8" s="7" t="s">
         <v>54</v>
       </c>
@@ -1327,8 +1331,9 @@
       <c r="E22" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
winch functions: cyrpus digial 1-2, cyrpus analog 1
</commit_message>
<xml_diff>
--- a/outputs.xlsx
+++ b/outputs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
   <si>
     <t>Hardware Summary</t>
   </si>
@@ -156,9 +156,6 @@
     <t>**: The compressor uses "compressor relay channel" 1</t>
   </si>
   <si>
-    <t>winch lock</t>
-  </si>
-  <si>
     <t>Decide which autonomous program to run</t>
   </si>
   <si>
@@ -184,6 +181,33 @@
   </si>
   <si>
     <t>On Cyprus</t>
+  </si>
+  <si>
+    <t>Winch Lock</t>
+  </si>
+  <si>
+    <t>CYPRUS STUFF</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Hold to fire winch</t>
+  </si>
+  <si>
+    <t>Push to lock / unlock</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Dial</t>
+  </si>
+  <si>
+    <t>Change winch speed</t>
   </si>
 </sst>
 </file>
@@ -566,7 +590,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -587,7 +611,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="9"/>
@@ -679,7 +703,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>7</v>
@@ -691,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -798,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -933,7 +957,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1112,7 +1136,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1132,7 +1156,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1166,7 +1190,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1233,17 +1257,17 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1271,50 +1295,90 @@
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="7">
+        <v>3</v>
+      </c>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="C14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4</v>
+      </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="7">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="7">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7"/>

</xml_diff>

<commit_message>
2 kicking powers, a third button to kick.
</commit_message>
<xml_diff>
--- a/outputs.xlsx
+++ b/outputs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Hardware Summary</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>Change winch speed</t>
+  </si>
+  <si>
+    <t>3 Way Switch: Roller forwards or backwards?</t>
+  </si>
+  <si>
+    <t>Fire the kicker</t>
+  </si>
+  <si>
+    <t>Set the kicker to "Low Power"</t>
   </si>
 </sst>
 </file>
@@ -266,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -292,6 +301,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,7 +1148,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E13" sqref="E13:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1333,7 +1345,9 @@
       <c r="D13" s="7">
         <v>3</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="12" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7"/>
@@ -1344,7 +1358,7 @@
       <c r="D14" s="7">
         <v>4</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="7"/>
@@ -1355,6 +1369,9 @@
       <c r="D15" s="7">
         <v>5</v>
       </c>
+      <c r="E15" s="6" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="7"/>
@@ -1364,6 +1381,9 @@
       </c>
       <c r="D16" s="7">
         <v>6</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1395,10 +1415,12 @@
       <c r="E22" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E13:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>